<commit_message>
Requirements and User stories docs
</commit_message>
<xml_diff>
--- a/מסמך דרישות.xlsx
+++ b/מסמך דרישות.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>מורה יוכל לצפות בתשובות התלמידים ולתת פידבק</t>
+  </si>
+  <si>
+    <t>מורה יוכל להגביל את מספר המילים בתשובה</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,9 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3">

</xml_diff>